<commit_message>
chalta hai ye sab
</commit_message>
<xml_diff>
--- a/public/reports/class_summary.xlsx
+++ b/public/reports/class_summary.xlsx
@@ -472,18 +472,18 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Understanding the hierarchical relationship and metallurgical requirements, Incomplete and imprecise explanation of calorific value and its affecting factors, Incomplete and inaccurate description of cracking types</t>
+          <t>Understanding the nuanced difference between 'caking coal' and 'coking coal', Incomplete and inaccurate description of cracking types, Incomplete and inaccurate explanation of factors affecting calorific value</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>

</xml_diff>